<commit_message>
Auto-committed on 2022/05/16 週一 11:51:46.03
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/L3-帳務作業/LoanRateChange.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/L3-帳務作業/LoanRateChange.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\SKL\DB\GenTables\L3-帳務作業\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCDF5C8F-3007-4945-B9F2-62882D86E265}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B4A0083-1C77-45AF-ABBB-DC1674B3BB69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DBD" sheetId="1" r:id="rId1"/>
@@ -705,6 +705,9 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -724,9 +727,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1069,8 +1069,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.44140625" defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -1087,10 +1087,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="28"/>
+      <c r="B1" s="29"/>
       <c r="C1" s="13" t="s">
         <v>64</v>
       </c>
@@ -1105,8 +1105,8 @@
       <c r="J1" s="22"/>
     </row>
     <row r="2" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="27"/>
-      <c r="B2" s="28"/>
+      <c r="A2" s="28"/>
+      <c r="B2" s="29"/>
       <c r="C2" s="11" t="s">
         <v>7</v>
       </c>
@@ -1121,10 +1121,10 @@
       <c r="J2" s="22"/>
     </row>
     <row r="3" spans="1:10" ht="32.4" x14ac:dyDescent="0.3">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="32"/>
+      <c r="B3" s="33"/>
       <c r="C3" s="16" t="s">
         <v>62</v>
       </c>
@@ -1139,10 +1139,10 @@
       <c r="J3" s="22"/>
     </row>
     <row r="4" spans="1:10" ht="42" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="31"/>
+      <c r="B4" s="32"/>
       <c r="C4" s="16" t="s">
         <v>87</v>
       </c>
@@ -1157,10 +1157,10 @@
       <c r="J4" s="22"/>
     </row>
     <row r="5" spans="1:10" ht="32.4" x14ac:dyDescent="0.3">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="32"/>
+      <c r="B5" s="33"/>
       <c r="C5" s="8" t="s">
         <v>91</v>
       </c>
@@ -1173,10 +1173,10 @@
       <c r="J5" s="22"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="30"/>
+      <c r="B6" s="31"/>
       <c r="C6" s="7"/>
       <c r="D6" s="23"/>
       <c r="E6" s="21"/>
@@ -1187,10 +1187,10 @@
       <c r="J6" s="22"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="31"/>
+      <c r="B7" s="32"/>
       <c r="C7" s="7"/>
       <c r="D7" s="23"/>
       <c r="E7" s="21"/>
@@ -1675,16 +1675,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.88671875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="109.77734375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="26.88671875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="43.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="130" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="58" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1781,8 +1781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C24C5444-93D8-4BDE-8D5A-69477DD64144}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="26.44140625" defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -1795,17 +1795,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="34" t="s">
         <v>100</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="26">
@@ -1823,7 +1823,7 @@
       <c r="E2" s="25">
         <v>8</v>
       </c>
-      <c r="F2" s="34" t="s">
+      <c r="F2" s="27" t="s">
         <v>105</v>
       </c>
       <c r="G2" s="24"/>

</xml_diff>